<commit_message>
se elimino una celda adicional
</commit_message>
<xml_diff>
--- a/procesamiento_variables/tabla_Ra_N.xlsx
+++ b/procesamiento_variables/tabla_Ra_N.xlsx
@@ -217,7 +217,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -341,15 +341,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z33"/>
+  <dimension ref="A1:Y33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z1" activeCellId="0" sqref="Z1"/>
+      <selection pane="topLeft" activeCell="W1" activeCellId="0" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="1" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="1" style="1" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -419,14 +419,13 @@
       <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2"/>
-      <c r="X1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -497,14 +496,13 @@
       <c r="V2" s="7" t="n">
         <v>11.462</v>
       </c>
-      <c r="W2" s="7"/>
-      <c r="X2" s="8" t="n">
+      <c r="W2" s="8" t="n">
         <v>31.851</v>
       </c>
-      <c r="Y2" s="7" t="n">
+      <c r="X2" s="7" t="n">
         <v>11.21</v>
       </c>
-      <c r="Z2" s="9" t="n">
+      <c r="Y2" s="9" t="n">
         <v>29.273</v>
       </c>
     </row>
@@ -575,14 +573,13 @@
       <c r="V3" s="7" t="n">
         <v>11.452</v>
       </c>
-      <c r="W3" s="7"/>
-      <c r="X3" s="8" t="n">
+      <c r="W3" s="8" t="n">
         <v>31.743</v>
       </c>
-      <c r="Y3" s="7" t="n">
+      <c r="X3" s="7" t="n">
         <v>11.205</v>
       </c>
-      <c r="Z3" s="9" t="n">
+      <c r="Y3" s="9" t="n">
         <v>29.219</v>
       </c>
     </row>
@@ -653,14 +650,13 @@
       <c r="V4" s="7" t="n">
         <v>11.441</v>
       </c>
-      <c r="W4" s="7"/>
-      <c r="X4" s="8" t="n">
+      <c r="W4" s="8" t="n">
         <v>31.636</v>
       </c>
-      <c r="Y4" s="7" t="n">
+      <c r="X4" s="7" t="n">
         <v>11.2</v>
       </c>
-      <c r="Z4" s="9" t="n">
+      <c r="Y4" s="9" t="n">
         <v>29.169</v>
       </c>
     </row>
@@ -731,14 +727,13 @@
       <c r="V5" s="7" t="n">
         <v>11.43</v>
       </c>
-      <c r="W5" s="7"/>
-      <c r="X5" s="8" t="n">
+      <c r="W5" s="8" t="n">
         <v>31.529</v>
       </c>
-      <c r="Y5" s="7" t="n">
+      <c r="X5" s="7" t="n">
         <v>11.195</v>
       </c>
-      <c r="Z5" s="9" t="n">
+      <c r="Y5" s="9" t="n">
         <v>29.121</v>
       </c>
     </row>
@@ -809,14 +804,13 @@
       <c r="V6" s="7" t="n">
         <v>11.419</v>
       </c>
-      <c r="W6" s="7"/>
-      <c r="X6" s="8" t="n">
+      <c r="W6" s="8" t="n">
         <v>31.424</v>
       </c>
-      <c r="Y6" s="7" t="n">
+      <c r="X6" s="7" t="n">
         <v>11.191</v>
       </c>
-      <c r="Z6" s="9" t="n">
+      <c r="Y6" s="9" t="n">
         <v>29.076</v>
       </c>
     </row>
@@ -887,14 +881,13 @@
       <c r="V7" s="7" t="n">
         <v>11.409</v>
       </c>
-      <c r="W7" s="7"/>
-      <c r="X7" s="8" t="n">
+      <c r="W7" s="8" t="n">
         <v>31.32</v>
       </c>
-      <c r="Y7" s="7" t="n">
+      <c r="X7" s="7" t="n">
         <v>11.187</v>
       </c>
-      <c r="Z7" s="9" t="n">
+      <c r="Y7" s="9" t="n">
         <v>29.034</v>
       </c>
     </row>
@@ -965,14 +958,13 @@
       <c r="V8" s="7" t="n">
         <v>11.399</v>
       </c>
-      <c r="W8" s="7"/>
-      <c r="X8" s="8" t="n">
+      <c r="W8" s="8" t="n">
         <v>31.217</v>
       </c>
-      <c r="Y8" s="7" t="n">
+      <c r="X8" s="7" t="n">
         <v>11.183</v>
       </c>
-      <c r="Z8" s="9" t="n">
+      <c r="Y8" s="9" t="n">
         <v>28.995</v>
       </c>
     </row>
@@ -1043,14 +1035,13 @@
       <c r="V9" s="7" t="n">
         <v>11.389</v>
       </c>
-      <c r="W9" s="7"/>
-      <c r="X9" s="8" t="n">
+      <c r="W9" s="8" t="n">
         <v>31.115</v>
       </c>
-      <c r="Y9" s="7" t="n">
+      <c r="X9" s="7" t="n">
         <v>11.179</v>
       </c>
-      <c r="Z9" s="9" t="n">
+      <c r="Y9" s="9" t="n">
         <v>28.958</v>
       </c>
     </row>
@@ -1121,14 +1112,13 @@
       <c r="V10" s="7" t="n">
         <v>11.379</v>
       </c>
-      <c r="W10" s="7"/>
-      <c r="X10" s="8" t="n">
+      <c r="W10" s="8" t="n">
         <v>31.015</v>
       </c>
-      <c r="Y10" s="7" t="n">
+      <c r="X10" s="7" t="n">
         <v>11.176</v>
       </c>
-      <c r="Z10" s="9" t="n">
+      <c r="Y10" s="9" t="n">
         <v>28.925</v>
       </c>
     </row>
@@ -1199,14 +1189,13 @@
       <c r="V11" s="7" t="n">
         <v>11.369</v>
       </c>
-      <c r="W11" s="7"/>
-      <c r="X11" s="8" t="n">
+      <c r="W11" s="8" t="n">
         <v>30.915</v>
       </c>
-      <c r="Y11" s="7" t="n">
+      <c r="X11" s="7" t="n">
         <v>11.173</v>
       </c>
-      <c r="Z11" s="9" t="n">
+      <c r="Y11" s="9" t="n">
         <v>28.894</v>
       </c>
     </row>
@@ -1277,14 +1266,13 @@
       <c r="V12" s="7" t="n">
         <v>11.359</v>
       </c>
-      <c r="W12" s="7"/>
-      <c r="X12" s="8" t="n">
+      <c r="W12" s="8" t="n">
         <v>30.831</v>
       </c>
-      <c r="Y12" s="7" t="n">
+      <c r="X12" s="7" t="n">
         <v>11.17</v>
       </c>
-      <c r="Z12" s="9" t="n">
+      <c r="Y12" s="9" t="n">
         <v>28.867</v>
       </c>
     </row>
@@ -1355,14 +1343,13 @@
       <c r="V13" s="7" t="n">
         <v>11.35</v>
       </c>
-      <c r="W13" s="7"/>
-      <c r="X13" s="8" t="n">
+      <c r="W13" s="8" t="n">
         <v>30.734</v>
       </c>
-      <c r="Y13" s="7" t="n">
+      <c r="X13" s="7" t="n">
         <v>11.168</v>
       </c>
-      <c r="Z13" s="9" t="n">
+      <c r="Y13" s="9" t="n">
         <v>28.842</v>
       </c>
     </row>
@@ -1433,14 +1420,13 @@
       <c r="V14" s="7" t="n">
         <v>11.341</v>
       </c>
-      <c r="W14" s="7"/>
-      <c r="X14" s="8" t="n">
+      <c r="W14" s="8" t="n">
         <v>30.639</v>
       </c>
-      <c r="Y14" s="7" t="n">
+      <c r="X14" s="7" t="n">
         <v>11.165</v>
       </c>
-      <c r="Z14" s="9" t="n">
+      <c r="Y14" s="9" t="n">
         <v>28.82</v>
       </c>
     </row>
@@ -1511,14 +1497,13 @@
       <c r="V15" s="7" t="n">
         <v>11.332</v>
       </c>
-      <c r="W15" s="7"/>
-      <c r="X15" s="8" t="n">
+      <c r="W15" s="8" t="n">
         <v>30.546</v>
       </c>
-      <c r="Y15" s="7" t="n">
+      <c r="X15" s="7" t="n">
         <v>11.164</v>
       </c>
-      <c r="Z15" s="9" t="n">
+      <c r="Y15" s="9" t="n">
         <v>28.802</v>
       </c>
     </row>
@@ -1589,14 +1574,13 @@
       <c r="V16" s="7" t="n">
         <v>11.323</v>
       </c>
-      <c r="W16" s="7"/>
-      <c r="X16" s="8" t="n">
+      <c r="W16" s="8" t="n">
         <v>30.454</v>
       </c>
-      <c r="Y16" s="7" t="n">
+      <c r="X16" s="7" t="n">
         <v>11.162</v>
       </c>
-      <c r="Z16" s="9" t="n">
+      <c r="Y16" s="9" t="n">
         <v>28.786</v>
       </c>
     </row>
@@ -1667,14 +1651,13 @@
       <c r="V17" s="7" t="n">
         <v>11.314</v>
       </c>
-      <c r="W17" s="7"/>
-      <c r="X17" s="8" t="n">
+      <c r="W17" s="8" t="n">
         <v>30.364</v>
       </c>
-      <c r="Y17" s="7" t="n">
+      <c r="X17" s="7" t="n">
         <v>11.161</v>
       </c>
-      <c r="Z17" s="9" t="n">
+      <c r="Y17" s="9" t="n">
         <v>28.774</v>
       </c>
     </row>
@@ -1745,14 +1728,13 @@
       <c r="V18" s="7" t="n">
         <v>11.306</v>
       </c>
-      <c r="W18" s="7"/>
-      <c r="X18" s="8" t="n">
+      <c r="W18" s="8" t="n">
         <v>30.276</v>
       </c>
-      <c r="Y18" s="7" t="n">
+      <c r="X18" s="7" t="n">
         <v>11.159</v>
       </c>
-      <c r="Z18" s="9" t="n">
+      <c r="Y18" s="9" t="n">
         <v>28.764</v>
       </c>
     </row>
@@ -1823,14 +1805,13 @@
       <c r="V19" s="7" t="n">
         <v>11.298</v>
       </c>
-      <c r="W19" s="7"/>
-      <c r="X19" s="8" t="n">
+      <c r="W19" s="8" t="n">
         <v>30.19</v>
       </c>
-      <c r="Y19" s="7" t="n">
+      <c r="X19" s="7" t="n">
         <v>11.159</v>
       </c>
-      <c r="Z19" s="9" t="n">
+      <c r="Y19" s="9" t="n">
         <v>28.758</v>
       </c>
     </row>
@@ -1901,14 +1882,13 @@
       <c r="V20" s="7" t="n">
         <v>11.289</v>
       </c>
-      <c r="W20" s="7"/>
-      <c r="X20" s="8" t="n">
+      <c r="W20" s="8" t="n">
         <v>30.106</v>
       </c>
-      <c r="Y20" s="7" t="n">
+      <c r="X20" s="7" t="n">
         <v>11.158</v>
       </c>
-      <c r="Z20" s="9" t="n">
+      <c r="Y20" s="9" t="n">
         <v>28.754</v>
       </c>
     </row>
@@ -1979,14 +1959,13 @@
       <c r="V21" s="7" t="n">
         <v>11.282</v>
       </c>
-      <c r="W21" s="7"/>
-      <c r="X21" s="8" t="n">
+      <c r="W21" s="8" t="n">
         <v>30.024</v>
       </c>
-      <c r="Y21" s="7" t="n">
+      <c r="X21" s="7" t="n">
         <v>11.158</v>
       </c>
-      <c r="Z21" s="9" t="n">
+      <c r="Y21" s="9" t="n">
         <v>28.754</v>
       </c>
     </row>
@@ -2057,14 +2036,13 @@
       <c r="V22" s="7" t="n">
         <v>11.274</v>
       </c>
-      <c r="W22" s="7"/>
-      <c r="X22" s="8" t="n">
+      <c r="W22" s="8" t="n">
         <v>29.944</v>
       </c>
-      <c r="Y22" s="7" t="n">
+      <c r="X22" s="7" t="n">
         <v>11.158</v>
       </c>
-      <c r="Z22" s="9" t="n">
+      <c r="Y22" s="9" t="n">
         <v>28.757</v>
       </c>
     </row>
@@ -2135,14 +2113,13 @@
       <c r="V23" s="7" t="n">
         <v>11.266</v>
       </c>
-      <c r="W23" s="7"/>
-      <c r="X23" s="8" t="n">
+      <c r="W23" s="8" t="n">
         <v>29.866</v>
       </c>
-      <c r="Y23" s="7" t="n">
+      <c r="X23" s="7" t="n">
         <v>11.158</v>
       </c>
-      <c r="Z23" s="9" t="n">
+      <c r="Y23" s="9" t="n">
         <v>28.763</v>
       </c>
     </row>
@@ -2213,14 +2190,13 @@
       <c r="V24" s="7" t="n">
         <v>11.259</v>
       </c>
-      <c r="W24" s="7"/>
-      <c r="X24" s="8" t="n">
+      <c r="W24" s="8" t="n">
         <v>29.791</v>
       </c>
-      <c r="Y24" s="7" t="n">
+      <c r="X24" s="7" t="n">
         <v>11.159</v>
       </c>
-      <c r="Z24" s="9" t="n">
+      <c r="Y24" s="9" t="n">
         <v>28.772</v>
       </c>
     </row>
@@ -2291,14 +2267,13 @@
       <c r="V25" s="7" t="n">
         <v>11.252</v>
       </c>
-      <c r="W25" s="7"/>
-      <c r="X25" s="8" t="n">
+      <c r="W25" s="8" t="n">
         <v>29.717</v>
       </c>
-      <c r="Y25" s="7" t="n">
+      <c r="X25" s="7" t="n">
         <v>11.159</v>
       </c>
-      <c r="Z25" s="9" t="n">
+      <c r="Y25" s="9" t="n">
         <v>28.784</v>
       </c>
     </row>
@@ -2369,14 +2344,13 @@
       <c r="V26" s="7" t="n">
         <v>11.245</v>
       </c>
-      <c r="W26" s="7"/>
-      <c r="X26" s="8" t="n">
+      <c r="W26" s="8" t="n">
         <v>29.647</v>
       </c>
-      <c r="Y26" s="7" t="n">
+      <c r="X26" s="7" t="n">
         <v>11.161</v>
       </c>
-      <c r="Z26" s="9" t="n">
+      <c r="Y26" s="9" t="n">
         <v>28.799</v>
       </c>
     </row>
@@ -2447,14 +2421,13 @@
       <c r="V27" s="7" t="n">
         <v>11.239</v>
       </c>
-      <c r="W27" s="7"/>
-      <c r="X27" s="8" t="n">
+      <c r="W27" s="8" t="n">
         <v>29.578</v>
       </c>
-      <c r="Y27" s="7" t="n">
+      <c r="X27" s="7" t="n">
         <v>11.162</v>
       </c>
-      <c r="Z27" s="9" t="n">
+      <c r="Y27" s="9" t="n">
         <v>28.818</v>
       </c>
     </row>
@@ -2525,14 +2498,13 @@
       <c r="V28" s="7" t="n">
         <v>11.233</v>
       </c>
-      <c r="W28" s="7"/>
-      <c r="X28" s="8" t="n">
+      <c r="W28" s="8" t="n">
         <v>29.512</v>
       </c>
-      <c r="Y28" s="7" t="n">
+      <c r="X28" s="7" t="n">
         <v>11.164</v>
       </c>
-      <c r="Z28" s="9" t="n">
+      <c r="Y28" s="9" t="n">
         <v>28.839</v>
       </c>
     </row>
@@ -2603,14 +2575,13 @@
       <c r="V29" s="7" t="n">
         <v>11.226</v>
       </c>
-      <c r="W29" s="7"/>
-      <c r="X29" s="8" t="n">
+      <c r="W29" s="8" t="n">
         <v>29.448</v>
       </c>
-      <c r="Y29" s="7" t="n">
+      <c r="X29" s="7" t="n">
         <v>11.166</v>
       </c>
-      <c r="Z29" s="9" t="n">
+      <c r="Y29" s="9" t="n">
         <v>28.863</v>
       </c>
     </row>
@@ -2681,14 +2652,13 @@
       <c r="V30" s="7" t="n">
         <v>11.221</v>
       </c>
-      <c r="W30" s="7"/>
-      <c r="X30" s="8" t="n">
+      <c r="W30" s="8" t="n">
         <v>29.387</v>
       </c>
-      <c r="Y30" s="7" t="n">
+      <c r="X30" s="7" t="n">
         <v>11.168</v>
       </c>
-      <c r="Z30" s="9" t="n">
+      <c r="Y30" s="9" t="n">
         <v>28.891</v>
       </c>
     </row>
@@ -2755,14 +2725,13 @@
       <c r="V31" s="7" t="n">
         <v>11.215</v>
       </c>
-      <c r="W31" s="7"/>
-      <c r="X31" s="8" t="n">
+      <c r="W31" s="8" t="n">
         <v>29.329</v>
       </c>
-      <c r="Y31" s="7" t="n">
+      <c r="X31" s="7" t="n">
         <v>11.17</v>
       </c>
-      <c r="Z31" s="9" t="n">
+      <c r="Y31" s="9" t="n">
         <v>28.921</v>
       </c>
     </row>
@@ -2816,11 +2785,10 @@
       </c>
       <c r="V32" s="11"/>
       <c r="W32" s="11"/>
-      <c r="X32" s="11"/>
-      <c r="Y32" s="7" t="n">
+      <c r="X32" s="7" t="n">
         <v>11.173</v>
       </c>
-      <c r="Z32" s="9" t="n">
+      <c r="Y32" s="9" t="n">
         <v>28.954</v>
       </c>
     </row>
@@ -2891,53 +2859,17 @@
       <c r="V33" s="12" t="n">
         <v>339.77</v>
       </c>
-      <c r="W33" s="12"/>
-      <c r="X33" s="13" t="n">
+      <c r="W33" s="13" t="n">
         <v>914.14</v>
       </c>
-      <c r="Y33" s="12" t="n">
+      <c r="X33" s="12" t="n">
         <v>346.31</v>
       </c>
-      <c r="Z33" s="14" t="n">
+      <c r="Y33" s="14" t="n">
         <v>895.74</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="V8:W8"/>
-    <mergeCell ref="V9:W9"/>
-    <mergeCell ref="V10:W10"/>
-    <mergeCell ref="V11:W11"/>
-    <mergeCell ref="V12:W12"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="V14:W14"/>
-    <mergeCell ref="V15:W15"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="V17:W17"/>
-    <mergeCell ref="V18:W18"/>
-    <mergeCell ref="V19:W19"/>
-    <mergeCell ref="V20:W20"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="V25:W25"/>
-    <mergeCell ref="V26:W26"/>
-    <mergeCell ref="V27:W27"/>
-    <mergeCell ref="V28:W28"/>
-    <mergeCell ref="V29:W29"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="V31:W31"/>
-    <mergeCell ref="V32:W32"/>
-    <mergeCell ref="V33:W33"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
se suben los notebooks
</commit_message>
<xml_diff>
--- a/procesamiento_variables/tabla_Ra_N.xlsx
+++ b/procesamiento_variables/tabla_Ra_N.xlsx
@@ -217,7 +217,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -341,15 +341,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z33"/>
+  <dimension ref="A1:Y33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z1" activeCellId="0" sqref="Z1"/>
+      <selection pane="topLeft" activeCell="W1" activeCellId="0" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="1" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="1" style="1" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -419,14 +419,13 @@
       <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2"/>
-      <c r="X1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -497,14 +496,13 @@
       <c r="V2" s="7" t="n">
         <v>11.462</v>
       </c>
-      <c r="W2" s="7"/>
-      <c r="X2" s="8" t="n">
+      <c r="W2" s="8" t="n">
         <v>31.851</v>
       </c>
-      <c r="Y2" s="7" t="n">
+      <c r="X2" s="7" t="n">
         <v>11.21</v>
       </c>
-      <c r="Z2" s="9" t="n">
+      <c r="Y2" s="9" t="n">
         <v>29.273</v>
       </c>
     </row>
@@ -575,14 +573,13 @@
       <c r="V3" s="7" t="n">
         <v>11.452</v>
       </c>
-      <c r="W3" s="7"/>
-      <c r="X3" s="8" t="n">
+      <c r="W3" s="8" t="n">
         <v>31.743</v>
       </c>
-      <c r="Y3" s="7" t="n">
+      <c r="X3" s="7" t="n">
         <v>11.205</v>
       </c>
-      <c r="Z3" s="9" t="n">
+      <c r="Y3" s="9" t="n">
         <v>29.219</v>
       </c>
     </row>
@@ -653,14 +650,13 @@
       <c r="V4" s="7" t="n">
         <v>11.441</v>
       </c>
-      <c r="W4" s="7"/>
-      <c r="X4" s="8" t="n">
+      <c r="W4" s="8" t="n">
         <v>31.636</v>
       </c>
-      <c r="Y4" s="7" t="n">
+      <c r="X4" s="7" t="n">
         <v>11.2</v>
       </c>
-      <c r="Z4" s="9" t="n">
+      <c r="Y4" s="9" t="n">
         <v>29.169</v>
       </c>
     </row>
@@ -731,14 +727,13 @@
       <c r="V5" s="7" t="n">
         <v>11.43</v>
       </c>
-      <c r="W5" s="7"/>
-      <c r="X5" s="8" t="n">
+      <c r="W5" s="8" t="n">
         <v>31.529</v>
       </c>
-      <c r="Y5" s="7" t="n">
+      <c r="X5" s="7" t="n">
         <v>11.195</v>
       </c>
-      <c r="Z5" s="9" t="n">
+      <c r="Y5" s="9" t="n">
         <v>29.121</v>
       </c>
     </row>
@@ -809,14 +804,13 @@
       <c r="V6" s="7" t="n">
         <v>11.419</v>
       </c>
-      <c r="W6" s="7"/>
-      <c r="X6" s="8" t="n">
+      <c r="W6" s="8" t="n">
         <v>31.424</v>
       </c>
-      <c r="Y6" s="7" t="n">
+      <c r="X6" s="7" t="n">
         <v>11.191</v>
       </c>
-      <c r="Z6" s="9" t="n">
+      <c r="Y6" s="9" t="n">
         <v>29.076</v>
       </c>
     </row>
@@ -887,14 +881,13 @@
       <c r="V7" s="7" t="n">
         <v>11.409</v>
       </c>
-      <c r="W7" s="7"/>
-      <c r="X7" s="8" t="n">
+      <c r="W7" s="8" t="n">
         <v>31.32</v>
       </c>
-      <c r="Y7" s="7" t="n">
+      <c r="X7" s="7" t="n">
         <v>11.187</v>
       </c>
-      <c r="Z7" s="9" t="n">
+      <c r="Y7" s="9" t="n">
         <v>29.034</v>
       </c>
     </row>
@@ -965,14 +958,13 @@
       <c r="V8" s="7" t="n">
         <v>11.399</v>
       </c>
-      <c r="W8" s="7"/>
-      <c r="X8" s="8" t="n">
+      <c r="W8" s="8" t="n">
         <v>31.217</v>
       </c>
-      <c r="Y8" s="7" t="n">
+      <c r="X8" s="7" t="n">
         <v>11.183</v>
       </c>
-      <c r="Z8" s="9" t="n">
+      <c r="Y8" s="9" t="n">
         <v>28.995</v>
       </c>
     </row>
@@ -1043,14 +1035,13 @@
       <c r="V9" s="7" t="n">
         <v>11.389</v>
       </c>
-      <c r="W9" s="7"/>
-      <c r="X9" s="8" t="n">
+      <c r="W9" s="8" t="n">
         <v>31.115</v>
       </c>
-      <c r="Y9" s="7" t="n">
+      <c r="X9" s="7" t="n">
         <v>11.179</v>
       </c>
-      <c r="Z9" s="9" t="n">
+      <c r="Y9" s="9" t="n">
         <v>28.958</v>
       </c>
     </row>
@@ -1121,14 +1112,13 @@
       <c r="V10" s="7" t="n">
         <v>11.379</v>
       </c>
-      <c r="W10" s="7"/>
-      <c r="X10" s="8" t="n">
+      <c r="W10" s="8" t="n">
         <v>31.015</v>
       </c>
-      <c r="Y10" s="7" t="n">
+      <c r="X10" s="7" t="n">
         <v>11.176</v>
       </c>
-      <c r="Z10" s="9" t="n">
+      <c r="Y10" s="9" t="n">
         <v>28.925</v>
       </c>
     </row>
@@ -1199,14 +1189,13 @@
       <c r="V11" s="7" t="n">
         <v>11.369</v>
       </c>
-      <c r="W11" s="7"/>
-      <c r="X11" s="8" t="n">
+      <c r="W11" s="8" t="n">
         <v>30.915</v>
       </c>
-      <c r="Y11" s="7" t="n">
+      <c r="X11" s="7" t="n">
         <v>11.173</v>
       </c>
-      <c r="Z11" s="9" t="n">
+      <c r="Y11" s="9" t="n">
         <v>28.894</v>
       </c>
     </row>
@@ -1277,14 +1266,13 @@
       <c r="V12" s="7" t="n">
         <v>11.359</v>
       </c>
-      <c r="W12" s="7"/>
-      <c r="X12" s="8" t="n">
+      <c r="W12" s="8" t="n">
         <v>30.831</v>
       </c>
-      <c r="Y12" s="7" t="n">
+      <c r="X12" s="7" t="n">
         <v>11.17</v>
       </c>
-      <c r="Z12" s="9" t="n">
+      <c r="Y12" s="9" t="n">
         <v>28.867</v>
       </c>
     </row>
@@ -1355,14 +1343,13 @@
       <c r="V13" s="7" t="n">
         <v>11.35</v>
       </c>
-      <c r="W13" s="7"/>
-      <c r="X13" s="8" t="n">
+      <c r="W13" s="8" t="n">
         <v>30.734</v>
       </c>
-      <c r="Y13" s="7" t="n">
+      <c r="X13" s="7" t="n">
         <v>11.168</v>
       </c>
-      <c r="Z13" s="9" t="n">
+      <c r="Y13" s="9" t="n">
         <v>28.842</v>
       </c>
     </row>
@@ -1433,14 +1420,13 @@
       <c r="V14" s="7" t="n">
         <v>11.341</v>
       </c>
-      <c r="W14" s="7"/>
-      <c r="X14" s="8" t="n">
+      <c r="W14" s="8" t="n">
         <v>30.639</v>
       </c>
-      <c r="Y14" s="7" t="n">
+      <c r="X14" s="7" t="n">
         <v>11.165</v>
       </c>
-      <c r="Z14" s="9" t="n">
+      <c r="Y14" s="9" t="n">
         <v>28.82</v>
       </c>
     </row>
@@ -1511,14 +1497,13 @@
       <c r="V15" s="7" t="n">
         <v>11.332</v>
       </c>
-      <c r="W15" s="7"/>
-      <c r="X15" s="8" t="n">
+      <c r="W15" s="8" t="n">
         <v>30.546</v>
       </c>
-      <c r="Y15" s="7" t="n">
+      <c r="X15" s="7" t="n">
         <v>11.164</v>
       </c>
-      <c r="Z15" s="9" t="n">
+      <c r="Y15" s="9" t="n">
         <v>28.802</v>
       </c>
     </row>
@@ -1589,14 +1574,13 @@
       <c r="V16" s="7" t="n">
         <v>11.323</v>
       </c>
-      <c r="W16" s="7"/>
-      <c r="X16" s="8" t="n">
+      <c r="W16" s="8" t="n">
         <v>30.454</v>
       </c>
-      <c r="Y16" s="7" t="n">
+      <c r="X16" s="7" t="n">
         <v>11.162</v>
       </c>
-      <c r="Z16" s="9" t="n">
+      <c r="Y16" s="9" t="n">
         <v>28.786</v>
       </c>
     </row>
@@ -1667,14 +1651,13 @@
       <c r="V17" s="7" t="n">
         <v>11.314</v>
       </c>
-      <c r="W17" s="7"/>
-      <c r="X17" s="8" t="n">
+      <c r="W17" s="8" t="n">
         <v>30.364</v>
       </c>
-      <c r="Y17" s="7" t="n">
+      <c r="X17" s="7" t="n">
         <v>11.161</v>
       </c>
-      <c r="Z17" s="9" t="n">
+      <c r="Y17" s="9" t="n">
         <v>28.774</v>
       </c>
     </row>
@@ -1745,14 +1728,13 @@
       <c r="V18" s="7" t="n">
         <v>11.306</v>
       </c>
-      <c r="W18" s="7"/>
-      <c r="X18" s="8" t="n">
+      <c r="W18" s="8" t="n">
         <v>30.276</v>
       </c>
-      <c r="Y18" s="7" t="n">
+      <c r="X18" s="7" t="n">
         <v>11.159</v>
       </c>
-      <c r="Z18" s="9" t="n">
+      <c r="Y18" s="9" t="n">
         <v>28.764</v>
       </c>
     </row>
@@ -1823,14 +1805,13 @@
       <c r="V19" s="7" t="n">
         <v>11.298</v>
       </c>
-      <c r="W19" s="7"/>
-      <c r="X19" s="8" t="n">
+      <c r="W19" s="8" t="n">
         <v>30.19</v>
       </c>
-      <c r="Y19" s="7" t="n">
+      <c r="X19" s="7" t="n">
         <v>11.159</v>
       </c>
-      <c r="Z19" s="9" t="n">
+      <c r="Y19" s="9" t="n">
         <v>28.758</v>
       </c>
     </row>
@@ -1901,14 +1882,13 @@
       <c r="V20" s="7" t="n">
         <v>11.289</v>
       </c>
-      <c r="W20" s="7"/>
-      <c r="X20" s="8" t="n">
+      <c r="W20" s="8" t="n">
         <v>30.106</v>
       </c>
-      <c r="Y20" s="7" t="n">
+      <c r="X20" s="7" t="n">
         <v>11.158</v>
       </c>
-      <c r="Z20" s="9" t="n">
+      <c r="Y20" s="9" t="n">
         <v>28.754</v>
       </c>
     </row>
@@ -1979,14 +1959,13 @@
       <c r="V21" s="7" t="n">
         <v>11.282</v>
       </c>
-      <c r="W21" s="7"/>
-      <c r="X21" s="8" t="n">
+      <c r="W21" s="8" t="n">
         <v>30.024</v>
       </c>
-      <c r="Y21" s="7" t="n">
+      <c r="X21" s="7" t="n">
         <v>11.158</v>
       </c>
-      <c r="Z21" s="9" t="n">
+      <c r="Y21" s="9" t="n">
         <v>28.754</v>
       </c>
     </row>
@@ -2057,14 +2036,13 @@
       <c r="V22" s="7" t="n">
         <v>11.274</v>
       </c>
-      <c r="W22" s="7"/>
-      <c r="X22" s="8" t="n">
+      <c r="W22" s="8" t="n">
         <v>29.944</v>
       </c>
-      <c r="Y22" s="7" t="n">
+      <c r="X22" s="7" t="n">
         <v>11.158</v>
       </c>
-      <c r="Z22" s="9" t="n">
+      <c r="Y22" s="9" t="n">
         <v>28.757</v>
       </c>
     </row>
@@ -2135,14 +2113,13 @@
       <c r="V23" s="7" t="n">
         <v>11.266</v>
       </c>
-      <c r="W23" s="7"/>
-      <c r="X23" s="8" t="n">
+      <c r="W23" s="8" t="n">
         <v>29.866</v>
       </c>
-      <c r="Y23" s="7" t="n">
+      <c r="X23" s="7" t="n">
         <v>11.158</v>
       </c>
-      <c r="Z23" s="9" t="n">
+      <c r="Y23" s="9" t="n">
         <v>28.763</v>
       </c>
     </row>
@@ -2213,14 +2190,13 @@
       <c r="V24" s="7" t="n">
         <v>11.259</v>
       </c>
-      <c r="W24" s="7"/>
-      <c r="X24" s="8" t="n">
+      <c r="W24" s="8" t="n">
         <v>29.791</v>
       </c>
-      <c r="Y24" s="7" t="n">
+      <c r="X24" s="7" t="n">
         <v>11.159</v>
       </c>
-      <c r="Z24" s="9" t="n">
+      <c r="Y24" s="9" t="n">
         <v>28.772</v>
       </c>
     </row>
@@ -2291,14 +2267,13 @@
       <c r="V25" s="7" t="n">
         <v>11.252</v>
       </c>
-      <c r="W25" s="7"/>
-      <c r="X25" s="8" t="n">
+      <c r="W25" s="8" t="n">
         <v>29.717</v>
       </c>
-      <c r="Y25" s="7" t="n">
+      <c r="X25" s="7" t="n">
         <v>11.159</v>
       </c>
-      <c r="Z25" s="9" t="n">
+      <c r="Y25" s="9" t="n">
         <v>28.784</v>
       </c>
     </row>
@@ -2369,14 +2344,13 @@
       <c r="V26" s="7" t="n">
         <v>11.245</v>
       </c>
-      <c r="W26" s="7"/>
-      <c r="X26" s="8" t="n">
+      <c r="W26" s="8" t="n">
         <v>29.647</v>
       </c>
-      <c r="Y26" s="7" t="n">
+      <c r="X26" s="7" t="n">
         <v>11.161</v>
       </c>
-      <c r="Z26" s="9" t="n">
+      <c r="Y26" s="9" t="n">
         <v>28.799</v>
       </c>
     </row>
@@ -2447,14 +2421,13 @@
       <c r="V27" s="7" t="n">
         <v>11.239</v>
       </c>
-      <c r="W27" s="7"/>
-      <c r="X27" s="8" t="n">
+      <c r="W27" s="8" t="n">
         <v>29.578</v>
       </c>
-      <c r="Y27" s="7" t="n">
+      <c r="X27" s="7" t="n">
         <v>11.162</v>
       </c>
-      <c r="Z27" s="9" t="n">
+      <c r="Y27" s="9" t="n">
         <v>28.818</v>
       </c>
     </row>
@@ -2525,14 +2498,13 @@
       <c r="V28" s="7" t="n">
         <v>11.233</v>
       </c>
-      <c r="W28" s="7"/>
-      <c r="X28" s="8" t="n">
+      <c r="W28" s="8" t="n">
         <v>29.512</v>
       </c>
-      <c r="Y28" s="7" t="n">
+      <c r="X28" s="7" t="n">
         <v>11.164</v>
       </c>
-      <c r="Z28" s="9" t="n">
+      <c r="Y28" s="9" t="n">
         <v>28.839</v>
       </c>
     </row>
@@ -2603,14 +2575,13 @@
       <c r="V29" s="7" t="n">
         <v>11.226</v>
       </c>
-      <c r="W29" s="7"/>
-      <c r="X29" s="8" t="n">
+      <c r="W29" s="8" t="n">
         <v>29.448</v>
       </c>
-      <c r="Y29" s="7" t="n">
+      <c r="X29" s="7" t="n">
         <v>11.166</v>
       </c>
-      <c r="Z29" s="9" t="n">
+      <c r="Y29" s="9" t="n">
         <v>28.863</v>
       </c>
     </row>
@@ -2681,14 +2652,13 @@
       <c r="V30" s="7" t="n">
         <v>11.221</v>
       </c>
-      <c r="W30" s="7"/>
-      <c r="X30" s="8" t="n">
+      <c r="W30" s="8" t="n">
         <v>29.387</v>
       </c>
-      <c r="Y30" s="7" t="n">
+      <c r="X30" s="7" t="n">
         <v>11.168</v>
       </c>
-      <c r="Z30" s="9" t="n">
+      <c r="Y30" s="9" t="n">
         <v>28.891</v>
       </c>
     </row>
@@ -2755,14 +2725,13 @@
       <c r="V31" s="7" t="n">
         <v>11.215</v>
       </c>
-      <c r="W31" s="7"/>
-      <c r="X31" s="8" t="n">
+      <c r="W31" s="8" t="n">
         <v>29.329</v>
       </c>
-      <c r="Y31" s="7" t="n">
+      <c r="X31" s="7" t="n">
         <v>11.17</v>
       </c>
-      <c r="Z31" s="9" t="n">
+      <c r="Y31" s="9" t="n">
         <v>28.921</v>
       </c>
     </row>
@@ -2816,11 +2785,10 @@
       </c>
       <c r="V32" s="11"/>
       <c r="W32" s="11"/>
-      <c r="X32" s="11"/>
-      <c r="Y32" s="7" t="n">
+      <c r="X32" s="7" t="n">
         <v>11.173</v>
       </c>
-      <c r="Z32" s="9" t="n">
+      <c r="Y32" s="9" t="n">
         <v>28.954</v>
       </c>
     </row>
@@ -2891,53 +2859,17 @@
       <c r="V33" s="12" t="n">
         <v>339.77</v>
       </c>
-      <c r="W33" s="12"/>
-      <c r="X33" s="13" t="n">
+      <c r="W33" s="13" t="n">
         <v>914.14</v>
       </c>
-      <c r="Y33" s="12" t="n">
+      <c r="X33" s="12" t="n">
         <v>346.31</v>
       </c>
-      <c r="Z33" s="14" t="n">
+      <c r="Y33" s="14" t="n">
         <v>895.74</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="V8:W8"/>
-    <mergeCell ref="V9:W9"/>
-    <mergeCell ref="V10:W10"/>
-    <mergeCell ref="V11:W11"/>
-    <mergeCell ref="V12:W12"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="V14:W14"/>
-    <mergeCell ref="V15:W15"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="V17:W17"/>
-    <mergeCell ref="V18:W18"/>
-    <mergeCell ref="V19:W19"/>
-    <mergeCell ref="V20:W20"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="V25:W25"/>
-    <mergeCell ref="V26:W26"/>
-    <mergeCell ref="V27:W27"/>
-    <mergeCell ref="V28:W28"/>
-    <mergeCell ref="V29:W29"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="V31:W31"/>
-    <mergeCell ref="V32:W32"/>
-    <mergeCell ref="V33:W33"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>